<commit_message>
Added eu region test cases
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh N\eclipse-workspace\BrevilleTest\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shanmsel\eclipse-workspace\BrevilleTest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7AF01C-955B-4766-8B7D-E114E4F53080}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0B00E258-C623-4AEC-B228-5960D0F273A8}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="23260" windowHeight="12580"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="46">
   <si>
     <t>TestCase</t>
   </si>
@@ -139,12 +138,45 @@
   </si>
   <si>
     <t>brevilleautomation02@yopmail.com.full</t>
+  </si>
+  <si>
+    <t>Place an Order For EU/DE region</t>
+  </si>
+  <si>
+    <t>eu</t>
+  </si>
+  <si>
+    <t>Mohrenstraße 30</t>
+  </si>
+  <si>
+    <t>Berlin</t>
+  </si>
+  <si>
+    <t>3020230011</t>
+  </si>
+  <si>
+    <t>Place an Order For UK region</t>
+  </si>
+  <si>
+    <t>uk</t>
+  </si>
+  <si>
+    <t>179-199 Holland Park Ave</t>
+  </si>
+  <si>
+    <t>London</t>
+  </si>
+  <si>
+    <t>W11 4UL</t>
+  </si>
+  <si>
+    <t>2076033355</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -223,7 +255,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -242,6 +274,8 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -556,29 +590,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2C1A8F3-5936-4D65-9AD5-55B8D209615F}">
-  <dimension ref="A1:N3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29.21875" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.453125" style="10" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -606,7 +642,7 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
@@ -622,7 +658,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
@@ -653,20 +689,20 @@
       <c r="J2" s="2">
         <v>3126211234</v>
       </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>31</v>
       </c>
@@ -700,7 +736,7 @@
       <c r="K3" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L3" s="11" t="s">
+      <c r="L3" s="13" t="s">
         <v>34</v>
       </c>
       <c r="M3" s="7" t="s">
@@ -710,41 +746,131 @@
         <v>32</v>
       </c>
     </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N5" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{5BF7D88E-52B8-414D-A47B-4800F130E8FC}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{99D27096-5991-48CD-8425-9E4366782E2C}"/>
-    <hyperlink ref="L3" r:id="rId3" xr:uid="{F905F1CB-618B-4B80-BA73-D48844CD79EA}"/>
+    <hyperlink ref="C5" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="L3" r:id="rId4"/>
+    <hyperlink ref="C2" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55305BA-B1C3-420C-B58E-747FBCCA4853}">
-  <dimension ref="A1:N6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="38" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -785,7 +911,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -826,7 +952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>18</v>
       </c>
@@ -867,7 +993,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>31</v>
       </c>
@@ -911,13 +1037,330 @@
         <v>32</v>
       </c>
     </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H13" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N13" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="2">
+        <v>60603</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J15" s="2">
+        <v>3126211234</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="2">
+        <v>4163611000</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H18" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="2">
+        <v>60603</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J21" s="2">
+        <v>3126211234</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N21" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J22" s="2">
+        <v>4163611000</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L22" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H23" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F6F81FFE-33C3-421C-BB37-68BBC77F610F}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{DCBB2621-F042-4BFF-B616-E22EE40CBD7B}"/>
-    <hyperlink ref="L2" r:id="rId3" xr:uid="{C452E3AC-DD8F-47E8-AD1E-A37FB15DF1F8}"/>
-    <hyperlink ref="C6" r:id="rId4" xr:uid="{C1F23A41-1523-4E47-B6C0-276AABDCDC7E}"/>
-    <hyperlink ref="L6" r:id="rId5" xr:uid="{189A3561-B0EC-4829-B27E-988B5AD71C50}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="L2" r:id="rId3"/>
+    <hyperlink ref="C6" r:id="rId4"/>
+    <hyperlink ref="L6" r:id="rId5"/>
+    <hyperlink ref="C13" r:id="rId6"/>
+    <hyperlink ref="C16" r:id="rId7"/>
+    <hyperlink ref="L16" r:id="rId8"/>
+    <hyperlink ref="C15" r:id="rId9"/>
+    <hyperlink ref="C18" r:id="rId10"/>
+    <hyperlink ref="C23" r:id="rId11"/>
+    <hyperlink ref="C22" r:id="rId12"/>
+    <hyperlink ref="L22" r:id="rId13"/>
+    <hyperlink ref="C21" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated Email Verification code
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh N\eclipse-workspace\BrevilleTest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB013BF6-C136-4CB2-B15F-A43B5017CD04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C73AEC-075D-4A98-980A-CA59BF985FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,9 @@
     <sheet name="US" sheetId="4" r:id="rId3"/>
     <sheet name="UK" sheetId="5" r:id="rId4"/>
     <sheet name="Demo" sheetId="7" r:id="rId5"/>
-    <sheet name="backup" sheetId="6" r:id="rId6"/>
+    <sheet name="ProdDemo" sheetId="8" r:id="rId6"/>
+    <sheet name="backup" sheetId="6" r:id="rId7"/>
+    <sheet name="Data" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="86">
   <si>
     <t>TestCase</t>
   </si>
@@ -188,25 +190,106 @@
     <t>Creditcard</t>
   </si>
   <si>
-    <t>cabreville0001@yopmail.com.full</t>
-  </si>
-  <si>
-    <t>usbrevilleuser0001@yopmail.com.full</t>
-  </si>
-  <si>
-    <t>Place one FG &amp; subscription order using paypalas a payment method from Breville and validate the order details in My Breville drop down - CA/FR</t>
-  </si>
-  <si>
     <t>Place one FG &amp; subscription order using credit card as payment method from Breville and validate the order details in My Breville drop down - CA/EN</t>
   </si>
   <si>
-    <t>Place one FG &amp; subscription order using paypalas a payment method from Breville and validate the order details in My Breville drop down - US/EN</t>
-  </si>
-  <si>
     <t>Place one FG &amp; subscription order using credit card as payment method from Breville and validate the order details in My Breville drop down - US/EN</t>
   </si>
   <si>
-    <t>ca.brevilleauto002@yopmail.com.full</t>
+    <t>Place one FG &amp; subscription order using credit card as payment method from Breville and validate the order details in My Breville drop down - UK/EN</t>
+  </si>
+  <si>
+    <t>ca.brevilleauto003@yopmail.com.full</t>
+  </si>
+  <si>
+    <t>us.brevilleauto002@yopmail.com.full</t>
+  </si>
+  <si>
+    <t>uk.brevilleauto001@yopmail.com.full</t>
+  </si>
+  <si>
+    <t>Aldwych</t>
+  </si>
+  <si>
+    <t>Place an Order For AU/EN region</t>
+  </si>
+  <si>
+    <t>Level 3/640 George St</t>
+  </si>
+  <si>
+    <t>Sydney</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>2895778675</t>
+  </si>
+  <si>
+    <t>creditcard</t>
+  </si>
+  <si>
+    <t>maheshtest85@gmail.com</t>
+  </si>
+  <si>
+    <t>maheshtest85@yahoo.com</t>
+  </si>
+  <si>
+    <t>mahesh.n86@yahoo.com</t>
+  </si>
+  <si>
+    <t>Place one FG &amp; subscription order using paypal as a payment method from Breville and validate the order details in My Breville drop down - CA/FR</t>
+  </si>
+  <si>
+    <t>Place one FG &amp; subscription order using paypal as a payment method from Breville and validate the order details in My Breville drop down - US/EN</t>
+  </si>
+  <si>
+    <t>Place one FG &amp; subscription order using paypal as a payment method from Breville and validate the order details in My Breville drop down - UK/EN</t>
+  </si>
+  <si>
+    <t>NewUser</t>
+  </si>
+  <si>
+    <t>Marsh Wall</t>
+  </si>
+  <si>
+    <t>E14 9SJ</t>
+  </si>
+  <si>
+    <t>Isle of Dogs</t>
+  </si>
+  <si>
+    <t>145 Richmond St W</t>
+  </si>
+  <si>
+    <t>M5H 2L2</t>
+  </si>
+  <si>
+    <t>Unit A</t>
+  </si>
+  <si>
+    <t>Place one FG &amp; subscription order using Credit card as a payment method from Breville and validate the order details in My Breville drop down - CA/FR</t>
+  </si>
+  <si>
+    <t>3900 S Las Vegas Blvd</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>Paypal</t>
+  </si>
+  <si>
+    <t>Place one FG &amp; subscription order using Paypal as a payment method from Breville and validate the order details in My Breville drop down - US/EN</t>
+  </si>
+  <si>
+    <t>eude</t>
+  </si>
+  <si>
+    <t>Stresemannstraße 36</t>
   </si>
 </sst>
 </file>
@@ -612,31 +695,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -683,233 +765,85 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>54</v>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="H2" s="2">
+        <v>10117</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
+      </c>
+      <c r="J2" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>52</v>
+        <v>71</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>30</v>
+        <v>85</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>51</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1" xr:uid="{56CCF987-8B4D-4B9F-9DFC-2E1356725C42}"/>
-    <hyperlink ref="L4" r:id="rId2" xr:uid="{296C632F-5A17-47D7-B1A6-B64F506075CD}"/>
-    <hyperlink ref="L5" r:id="rId3" xr:uid="{546B356B-8BE1-42CF-81CC-5BA2BFAAB2CF}"/>
-    <hyperlink ref="L2" r:id="rId4" xr:uid="{08DA0C39-9C25-4DCC-97E4-664C07283564}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDFC30B4-0CDC-49A3-8949-02307CB1E509}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -956,12 +890,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
@@ -991,7 +925,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>27</v>
@@ -1000,60 +934,12 @@
         <v>30</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="O3" s="4" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L3" r:id="rId1" xr:uid="{E4954566-E075-4FBF-8793-6553795B2162}"/>
-    <hyperlink ref="L2" r:id="rId2" xr:uid="{5BDDB207-B685-43F1-BB17-447B80CC23A9}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{B57ADED8-F8D2-45EC-A258-A1B8607F2A91}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1064,28 +950,27 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1132,9 +1017,9 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>18</v>
@@ -1167,7 +1052,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>27</v>
@@ -1179,9 +1064,9 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>18</v>
@@ -1214,7 +1099,7 @@
         <v>26</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>27</v>
@@ -1228,8 +1113,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{E2A29126-F804-4C08-95C9-1C60BFA3C2C1}"/>
-    <hyperlink ref="L3" r:id="rId2" xr:uid="{8B2FB97F-4D52-471A-AD70-F577ACC490FD}"/>
+    <hyperlink ref="L3" r:id="rId1" xr:uid="{7804F62E-6EBE-4974-AAC7-AB5E17A7D4FC}"/>
+    <hyperlink ref="L2" r:id="rId2" xr:uid="{95936762-76B6-4673-A56B-FDEBC75DD9AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1237,30 +1122,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F23363-2E6B-4A4C-8CDB-4414B6604A42}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1303,54 +1188,107 @@
       <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>38</v>
+      <c r="O1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="F3" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>28</v>
+      <c r="H3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CAC69271-DB33-4CEE-A47C-B3DA25FAC2CD}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{DFBC1C6A-99C5-4B08-B0D0-9953E8205E18}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1358,31 +1296,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5F83282-07AE-47A7-A5C5-54C7A96C76E5}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1429,12 +1366,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>55</v>
+        <v>68</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
@@ -1464,7 +1401,7 @@
         <v>26</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>27</v>
@@ -1473,43 +1410,283 @@
         <v>30</v>
       </c>
       <c r="O2" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="4" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="L2" r:id="rId1" xr:uid="{8E6ECA80-18DA-45B2-A6FB-0A544C0183C7}"/>
+    <hyperlink ref="L2" r:id="rId1" xr:uid="{D2004189-60DD-4010-B001-FC0EE2C094A9}"/>
+    <hyperlink ref="L3" r:id="rId2" xr:uid="{41080844-73A9-4305-9611-45B129C92098}"/>
+    <hyperlink ref="L5" r:id="rId3" xr:uid="{3BDB5D3A-AA90-4041-A8FD-68423ABC9560}"/>
+    <hyperlink ref="L4" r:id="rId4" xr:uid="{5AC5E59A-B9ED-4682-8F24-5CED0D664513}"/>
+    <hyperlink ref="L6" r:id="rId5" xr:uid="{D66C39EF-872D-4FA3-92FC-3C8B3C8B1367}"/>
+    <hyperlink ref="L7" r:id="rId6" xr:uid="{F8E2F39D-5A90-489D-8048-2AEB1BECC69B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD79AA9-1B12-49D7-80E7-72F36EBB72C6}">
-  <dimension ref="A1:N17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12B3FA48-946C-4947-BBFF-C6CA7A5B0C8E}">
+  <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="38.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.21875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.21875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.21875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1552,8 +1729,278 @@
       <c r="N1" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="O1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{62F98180-99E1-4412-8586-FCB3373A1597}"/>
+    <hyperlink ref="C5" r:id="rId2" xr:uid="{0E0232A4-B787-4425-BDFB-EE1F5A31A89B}"/>
+    <hyperlink ref="L2" r:id="rId3" xr:uid="{E59E851C-F2B7-4608-8FA3-F480CA92D0AA}"/>
+    <hyperlink ref="L3" r:id="rId4" xr:uid="{5ED6D01F-2E99-4E2B-ACFF-C7FFF25C6D3F}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DD79AA9-1B12-49D7-80E7-72F36EBB72C6}">
+  <dimension ref="A1:O87"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41:XFD41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1597,7 +2044,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>29</v>
       </c>
@@ -1641,7 +2088,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
@@ -1685,7 +2132,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>38</v>
       </c>
@@ -1729,7 +2176,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>44</v>
       </c>
@@ -1773,7 +2220,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>29</v>
       </c>
@@ -1817,7 +2264,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>44</v>
       </c>
@@ -1861,7 +2308,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1903,6 +2350,1322 @@
       </c>
       <c r="N17" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L25" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L26" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N26" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L27" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N27" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L30" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L39" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N39" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L40" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N40" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H41" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J41" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N41" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H42" s="2">
+        <v>2000</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="L42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N42" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L45" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M45" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N45" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A46" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L46" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M46" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L47" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M47" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N47" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K48" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L48" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N48" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K49" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L49" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M49" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K54" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L54" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="M54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J55" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L55" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M55" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N55" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L56" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M56" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N56" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L57" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N57" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J58" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L58" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M58" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N58" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A63" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J63" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="M63" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N63" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B69" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G69" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H69" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J69" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K69" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L69" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M69" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N69" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O69" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A72" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C72" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J72" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K72" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M72" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N72" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O72" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J75" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L75" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M75" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N75" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O75" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D79" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G79" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H79" s="2">
+        <v>89119</v>
+      </c>
+      <c r="I79" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J79" s="2">
+        <v>7022624000</v>
+      </c>
+      <c r="K79" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L79" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M79" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N79" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O79" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C80" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G80" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I80" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J80" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L80" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M80" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N80" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O80" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G81" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J81" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M81" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N81" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A85" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H85" s="2">
+        <v>89119</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J85" s="2">
+        <v>7022624000</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M85" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N85" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O85" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I86" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J86" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L86" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N86" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O86" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G87" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H87" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I87" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J87" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K87" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L87" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M87" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N87" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O87" s="4" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1916,7 +3679,244 @@
     <hyperlink ref="L15" r:id="rId7" xr:uid="{ABF12A9C-D9B3-4440-84BC-79F74D587C4C}"/>
     <hyperlink ref="L16" r:id="rId8" xr:uid="{E01AF184-3430-48A3-AEEF-4E3F540E5CFA}"/>
     <hyperlink ref="C17" r:id="rId9" xr:uid="{BB944C0D-38C7-4B13-B909-52B26885A6BF}"/>
+    <hyperlink ref="L25" r:id="rId10" xr:uid="{F5870F57-3593-4B4F-BB7B-F8B3C2600321}"/>
+    <hyperlink ref="L27" r:id="rId11" xr:uid="{C6BFB38D-9552-4AFA-8565-E10A7DADFD0A}"/>
+    <hyperlink ref="L26" r:id="rId12" xr:uid="{186146D1-683D-411F-8CEF-63DAC92DC1E6}"/>
+    <hyperlink ref="L30" r:id="rId13" xr:uid="{0E6F7DD1-E485-4B0F-9930-8EB8D29A5FB1}"/>
+    <hyperlink ref="C41" r:id="rId14" xr:uid="{0851479E-6471-401C-83EA-8CEA63F09820}"/>
+    <hyperlink ref="C42" r:id="rId15" xr:uid="{AC3FB595-25A9-4977-A45F-32BD517DF1CA}"/>
+    <hyperlink ref="L40" r:id="rId16" xr:uid="{9A756B6E-689F-4491-8CD5-5B1F23AC6011}"/>
+    <hyperlink ref="L39" r:id="rId17" xr:uid="{B233EB0C-1757-4359-91D9-3015369E7285}"/>
+    <hyperlink ref="L45" r:id="rId18" xr:uid="{1C415CB8-98AF-414F-9566-4105BAE3E482}"/>
+    <hyperlink ref="L47" r:id="rId19" xr:uid="{F4CF2E2B-BF93-4A80-9BC3-9DFE63824EF0}"/>
+    <hyperlink ref="L46" r:id="rId20" xr:uid="{A5AA2C87-B21A-4F6C-9BC0-BBCD921B434A}"/>
+    <hyperlink ref="L48" r:id="rId21" xr:uid="{4452F2A4-FF30-4152-92E2-1DC60CFDCB56}"/>
+    <hyperlink ref="L49" r:id="rId22" xr:uid="{A6679115-C88E-49B7-A00E-66CC0D16F149}"/>
+    <hyperlink ref="L54" r:id="rId23" xr:uid="{D00A41C5-51CC-4E06-9091-8489F1B686DB}"/>
+    <hyperlink ref="L56" r:id="rId24" xr:uid="{B1F1D8F9-C63B-41FC-8E91-5206FA8A57E6}"/>
+    <hyperlink ref="L55" r:id="rId25" xr:uid="{1879E120-D888-4670-A134-6C3E565C6F89}"/>
+    <hyperlink ref="L57" r:id="rId26" xr:uid="{A5DAF914-8EE2-4710-B863-712F26FE00AF}"/>
+    <hyperlink ref="L58" r:id="rId27" xr:uid="{D8E425B5-544B-4079-AD64-02D7DA444317}"/>
+    <hyperlink ref="L63" r:id="rId28" xr:uid="{0DD16F69-E993-4DEC-94E1-8845C76F602A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916E424B-CB2B-4001-A960-BD26F7B021CE}">
+  <dimension ref="A1:O4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.42578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="2">
+        <v>89119</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7022624000</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added D365 API test cases
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mahesh N\eclipse-workspace\BrevilleTest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3C73AEC-075D-4A98-980A-CA59BF985FA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F470B308-AA5F-4886-9950-0D197698E6ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="991" uniqueCount="87">
   <si>
     <t>TestCase</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>Stresemannstraße 36</t>
+  </si>
+  <si>
+    <t>111 West Adams Street</t>
   </si>
 </sst>
 </file>
@@ -698,7 +701,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,12 +768,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>33</v>
+    <row r="2" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>28</v>
@@ -782,34 +785,34 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>35</v>
+        <v>86</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="H2" s="2">
-        <v>10117</v>
+        <v>60603</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="J2" s="2">
+        <v>7022624000</v>
       </c>
       <c r="K2" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>85</v>
+        <v>30</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -950,7 +953,7 @@
   <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1299,7 +1302,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1937,7 +1940,7 @@
   <dimension ref="A1:O87"/>
   <sheetViews>
     <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+      <selection activeCell="O46" sqref="O46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3705,10 +3708,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{916E424B-CB2B-4001-A960-BD26F7B021CE}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3916,6 +3919,288 @@
         <v>51</v>
       </c>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="2">
+        <v>10117</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K9" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N9" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="2">
+        <v>89119</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="2">
+        <v>7022624000</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="2">
+        <v>4168693456</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="2">
+        <v>8712220042</v>
+      </c>
+      <c r="K15" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="2">
+        <v>89119</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="2">
+        <v>7022624000</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated beanz Testcases scenarios
</commit_message>
<xml_diff>
--- a/testdata/testData.xlsx
+++ b/testdata/testData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Breville_Automation\BrevilleTest\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13F0FF73-E0B3-4E64-90F6-AD5B9DEF32C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20B88ECC-7DF8-43A7-AB65-A5255D7FCD7E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,26 +17,17 @@
     <sheet name="D_365" sheetId="10" r:id="rId2"/>
     <sheet name="Backup" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="113">
   <si>
     <t>TestCase</t>
   </si>
@@ -368,10 +359,13 @@
     <t>A</t>
   </si>
   <si>
-    <t>Guest</t>
-  </si>
-  <si>
     <t>Lakshmi@yopmail.com</t>
+  </si>
+  <si>
+    <t>Every</t>
+  </si>
+  <si>
+    <t>Once a month</t>
   </si>
 </sst>
 </file>
@@ -417,7 +411,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -440,12 +434,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -483,6 +488,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -800,10 +808,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y2"/>
+  <dimension ref="A1:Z2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="38.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.453125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.81640625" customWidth="1"/>
+    <col min="17" max="17" width="15.81640625" style="6" customWidth="1"/>
+    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.26953125" style="6" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.1796875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.35">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="U1" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y1" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z1" s="17" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26" ht="58" x14ac:dyDescent="0.35">
+      <c r="A2" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="12">
+        <v>60603</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="12">
+        <v>7022624000</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="13" t="b">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="R2" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="S2" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="T2" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="U2" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y2" s="12">
+        <v>77060</v>
+      </c>
+      <c r="Z2" s="12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{F0F38653-CF45-461C-89BD-6838BAFA9D37}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1DEA2FA-25E2-4719-80B1-F25796A73B16}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="29.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>265823</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA78D756-01DD-4738-B827-13CB06D38CEF}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83D3F8-F256-4F35-89C0-A9D89387D36C}">
+  <dimension ref="A1:Y15"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -915,261 +1185,6 @@
         <v>41</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="12">
-        <v>60603</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="12">
-        <v>7022624000</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P2" s="13" t="b">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="R2" s="13" t="s">
-        <v>104</v>
-      </c>
-      <c r="S2" s="13" t="s">
-        <v>105</v>
-      </c>
-      <c r="T2" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="U2" s="15" t="s">
-        <v>107</v>
-      </c>
-      <c r="V2" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="W2" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="X2" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" s="12">
-        <v>77060</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F0F38653-CF45-461C-89BD-6838BAFA9D37}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1DEA2FA-25E2-4719-80B1-F25796A73B16}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="2" max="2" width="29.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.54296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="b">
-        <v>1</v>
-      </c>
-      <c r="E2" s="2">
-        <v>265823</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DA78D756-01DD-4738-B827-13CB06D38CEF}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF83D3F8-F256-4F35-89C0-A9D89387D36C}">
-  <dimension ref="A1:Y15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="38.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.7265625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.54296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.453125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="21.453125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.81640625" customWidth="1"/>
-    <col min="17" max="17" width="15.81640625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.7265625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="18.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.453125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.1796875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="P1" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="R1" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="S1" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="U1" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="W1" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="X1" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="Y1" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="12" t="s">

</xml_diff>